<commit_message>
Fixed minor mistake with construction of state variable, results only changed marginally
</commit_message>
<xml_diff>
--- a/Results/results_men.xlsx
+++ b/Results/results_men.xlsx
@@ -409,22 +409,22 @@
         </is>
       </c>
       <c r="C2">
-        <v>3.367868672252386</v>
+        <v>3.366303623731205</v>
       </c>
       <c r="D2">
-        <v>12.16990540133703</v>
+        <v>12.15714401385543</v>
       </c>
       <c r="E2">
-        <v>1.748999122802654</v>
+        <v>1.737188663037162</v>
       </c>
       <c r="F2">
-        <v>4.015623133956952</v>
+        <v>4.004564280816123</v>
       </c>
       <c r="G2">
-        <v>3.653626624253504</v>
+        <v>3.652049221412493</v>
       </c>
       <c r="H2">
-        <v>24.95602295460252</v>
+        <v>24.91724980285242</v>
       </c>
     </row>
     <row r="3">
@@ -437,22 +437,22 @@
         </is>
       </c>
       <c r="C3">
-        <v>4.687858192783213</v>
+        <v>4.686592407434943</v>
       </c>
       <c r="D3">
-        <v>12.72893382937644</v>
+        <v>12.74007630712849</v>
       </c>
       <c r="E3">
-        <v>1.063861653108825</v>
+        <v>1.067978942660879</v>
       </c>
       <c r="F3">
-        <v>5.827251758032741</v>
+        <v>5.785149508426985</v>
       </c>
       <c r="G3">
-        <v>4.642812936485146</v>
+        <v>4.629681100983577</v>
       </c>
       <c r="H3">
-        <v>28.95071836978637</v>
+        <v>28.90947826663487</v>
       </c>
     </row>
     <row r="4">
@@ -465,22 +465,22 @@
         </is>
       </c>
       <c r="C4">
-        <v>7.665543233338088</v>
+        <v>7.655722422417413</v>
       </c>
       <c r="D4">
-        <v>11.32905560485243</v>
+        <v>11.33642055198433</v>
       </c>
       <c r="E4">
-        <v>0.8763055175210696</v>
+        <v>0.8619887241378588</v>
       </c>
       <c r="F4">
-        <v>9.627423182790858</v>
+        <v>9.6321956492387</v>
       </c>
       <c r="G4">
-        <v>4.471843512311404</v>
+        <v>4.461747400534877</v>
       </c>
       <c r="H4">
-        <v>33.97017105081385</v>
+        <v>33.94807474831318</v>
       </c>
     </row>
     <row r="5">
@@ -493,22 +493,22 @@
         </is>
       </c>
       <c r="C5">
-        <v>3.062187206200391</v>
+        <v>3.056804037521745</v>
       </c>
       <c r="D5">
-        <v>11.30095906580892</v>
+        <v>11.28969770140409</v>
       </c>
       <c r="E5">
-        <v>2.706645495897704</v>
+        <v>2.634483856901404</v>
       </c>
       <c r="F5">
-        <v>3.353420684764564</v>
+        <v>3.383079511480429</v>
       </c>
       <c r="G5">
-        <v>2.508064306596661</v>
+        <v>2.530826876317968</v>
       </c>
       <c r="H5">
-        <v>22.93127675926824</v>
+        <v>22.89489198362563</v>
       </c>
     </row>
     <row r="6">
@@ -521,22 +521,22 @@
         </is>
       </c>
       <c r="C6">
-        <v>4.431000551283574</v>
+        <v>4.419344227387025</v>
       </c>
       <c r="D6">
-        <v>12.08223028587142</v>
+        <v>12.08477614690689</v>
       </c>
       <c r="E6">
-        <v>1.755952070960252</v>
+        <v>1.72254167945185</v>
       </c>
       <c r="F6">
-        <v>5.155560254335901</v>
+        <v>5.157664722330637</v>
       </c>
       <c r="G6">
-        <v>3.447049066969249</v>
+        <v>3.462173094514133</v>
       </c>
       <c r="H6">
-        <v>26.87179222942039</v>
+        <v>26.84649987059054</v>
       </c>
     </row>
     <row r="7">
@@ -549,22 +549,22 @@
         </is>
       </c>
       <c r="C7">
-        <v>7.475683165440112</v>
+        <v>7.446834057065592</v>
       </c>
       <c r="D7">
-        <v>10.80519923755975</v>
+        <v>10.79877460733823</v>
       </c>
       <c r="E7">
-        <v>1.37209630337009</v>
+        <v>1.318006191099182</v>
       </c>
       <c r="F7">
-        <v>9.165953073943385</v>
+        <v>9.236016582842852</v>
       </c>
       <c r="G7">
-        <v>3.609379007778034</v>
+        <v>3.629350868742752</v>
       </c>
       <c r="H7">
-        <v>32.42831078809137</v>
+        <v>32.42898230708861</v>
       </c>
     </row>
     <row r="8">
@@ -577,22 +577,22 @@
         </is>
       </c>
       <c r="C8">
-        <v>3.512410025416218</v>
+        <v>3.510322822902935</v>
       </c>
       <c r="D8">
-        <v>12.84238692927475</v>
+        <v>12.84694702643727</v>
       </c>
       <c r="E8">
-        <v>3.225850313468367</v>
+        <v>3.168009596498625</v>
       </c>
       <c r="F8">
-        <v>5.083256173374033</v>
+        <v>5.071380750934225</v>
       </c>
       <c r="G8">
-        <v>4.181963915464646</v>
+        <v>4.196158676738227</v>
       </c>
       <c r="H8">
-        <v>28.84586735699801</v>
+        <v>28.79281887351128</v>
       </c>
     </row>
     <row r="9">
@@ -605,22 +605,22 @@
         </is>
       </c>
       <c r="C9">
-        <v>4.704392402361273</v>
+        <v>4.703387344963951</v>
       </c>
       <c r="D9">
-        <v>13.28980612490604</v>
+        <v>13.3255840515091</v>
       </c>
       <c r="E9">
-        <v>2.000159723119942</v>
+        <v>1.987108590042685</v>
       </c>
       <c r="F9">
-        <v>6.978543961086959</v>
+        <v>6.903454256657646</v>
       </c>
       <c r="G9">
-        <v>5.259728320323254</v>
+        <v>5.25270401146703</v>
       </c>
       <c r="H9">
-        <v>32.23263053179747</v>
+        <v>32.17223825464041</v>
       </c>
     </row>
     <row r="10">
@@ -633,22 +633,22 @@
         </is>
       </c>
       <c r="C10">
-        <v>7.337422161313886</v>
+        <v>7.33472612500473</v>
       </c>
       <c r="D10">
-        <v>11.66439789603192</v>
+        <v>11.70590648267642</v>
       </c>
       <c r="E10">
-        <v>1.722119163893992</v>
+        <v>1.709671881039287</v>
       </c>
       <c r="F10">
-        <v>10.74283897264594</v>
+        <v>10.67236643672631</v>
       </c>
       <c r="G10">
-        <v>5.058769508059869</v>
+        <v>5.045643801293241</v>
       </c>
       <c r="H10">
-        <v>36.5255477019456</v>
+        <v>36.46831472673999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results over time, confidence intervals
</commit_message>
<xml_diff>
--- a/Results/results_men.xlsx
+++ b/Results/results_men.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2.5%" sheetId="2" r:id="rId2"/>
+    <sheet name="97.5%" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,40 +362,45 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>education</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>race</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>retired.healthy</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>retired.unhealthy</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>not.working</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>working.healthy</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>working.unhealthy</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
@@ -401,254 +408,1796 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>White</t>
         </is>
       </c>
-      <c r="C2">
-        <v>3.366303623731205</v>
-      </c>
       <c r="D2">
-        <v>12.15714401385543</v>
+        <v>3.904439941756977</v>
       </c>
       <c r="E2">
-        <v>1.737188663037162</v>
+        <v>12.26654948744224</v>
       </c>
       <c r="F2">
-        <v>4.004564280816123</v>
+        <v>1.87422278962173</v>
       </c>
       <c r="G2">
-        <v>3.652049221412493</v>
+        <v>4.137377948188109</v>
       </c>
       <c r="H2">
-        <v>24.91724980285242</v>
+        <v>4.166967579395159</v>
+      </c>
+      <c r="I2">
+        <v>26.34955774640421</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>White</t>
         </is>
       </c>
-      <c r="C3">
-        <v>4.686592407434943</v>
-      </c>
       <c r="D3">
-        <v>12.74007630712849</v>
+        <v>5.282472245330411</v>
       </c>
       <c r="E3">
-        <v>1.067978942660879</v>
+        <v>12.03036059941171</v>
       </c>
       <c r="F3">
-        <v>5.785149508426985</v>
+        <v>0.9783160536678729</v>
       </c>
       <c r="G3">
-        <v>4.629681100983577</v>
+        <v>5.407482797024506</v>
       </c>
       <c r="H3">
-        <v>28.90947826663487</v>
+        <v>4.962665279703942</v>
+      </c>
+      <c r="I3">
+        <v>28.66129697513845</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>White</t>
         </is>
       </c>
-      <c r="C4">
-        <v>7.655722422417413</v>
-      </c>
       <c r="D4">
-        <v>11.33642055198433</v>
+        <v>7.752141919084989</v>
       </c>
       <c r="E4">
-        <v>0.8619887241378588</v>
+        <v>11.66136212753755</v>
       </c>
       <c r="F4">
-        <v>9.6321956492387</v>
+        <v>0.7543597005537398</v>
       </c>
       <c r="G4">
-        <v>4.461747400534877</v>
+        <v>8.263145924393408</v>
       </c>
       <c r="H4">
-        <v>33.94807474831318</v>
+        <v>4.236252484246125</v>
+      </c>
+      <c r="I4">
+        <v>32.66726215581581</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Black</t>
         </is>
       </c>
-      <c r="C5">
-        <v>3.056804037521745</v>
-      </c>
       <c r="D5">
-        <v>11.28969770140409</v>
+        <v>3.90242357800833</v>
       </c>
       <c r="E5">
-        <v>2.634483856901404</v>
+        <v>10.4405824175149</v>
       </c>
       <c r="F5">
-        <v>3.383079511480429</v>
+        <v>2.906423535002142</v>
       </c>
       <c r="G5">
-        <v>2.530826876317968</v>
+        <v>4.565452737902664</v>
       </c>
       <c r="H5">
-        <v>22.89489198362563</v>
+        <v>2.525629007026098</v>
+      </c>
+      <c r="I5">
+        <v>24.34051127545414</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>Black</t>
         </is>
       </c>
-      <c r="C6">
-        <v>4.419344227387025</v>
-      </c>
       <c r="D6">
-        <v>12.08477614690689</v>
+        <v>5.421912341190843</v>
       </c>
       <c r="E6">
-        <v>1.72254167945185</v>
+        <v>10.53410914496424</v>
       </c>
       <c r="F6">
-        <v>5.157664722330637</v>
+        <v>1.786985949083931</v>
       </c>
       <c r="G6">
-        <v>3.462173094514133</v>
+        <v>5.530642879347573</v>
       </c>
       <c r="H6">
-        <v>26.84649987059054</v>
+        <v>3.08699906278645</v>
+      </c>
+      <c r="I6">
+        <v>26.36064937737304</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>Black</t>
         </is>
       </c>
-      <c r="C7">
-        <v>7.446834057065592</v>
-      </c>
       <c r="D7">
-        <v>10.79877460733823</v>
+        <v>7.919136326772108</v>
       </c>
       <c r="E7">
-        <v>1.318006191099182</v>
+        <v>10.12364976780039</v>
       </c>
       <c r="F7">
-        <v>9.236016582842852</v>
+        <v>1.143307876627796</v>
       </c>
       <c r="G7">
-        <v>3.629350868742752</v>
+        <v>9.062663087437013</v>
       </c>
       <c r="H7">
-        <v>32.42898230708861</v>
+        <v>2.83692146114122</v>
+      </c>
+      <c r="I7">
+        <v>31.08567851977853</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Hispanic</t>
         </is>
       </c>
-      <c r="C8">
-        <v>3.510322822902935</v>
-      </c>
       <c r="D8">
-        <v>12.84694702643727</v>
+        <v>3.834458114002897</v>
       </c>
       <c r="E8">
-        <v>3.168009596498625</v>
+        <v>12.64011474040511</v>
       </c>
       <c r="F8">
-        <v>5.071380750934225</v>
+        <v>2.838985644112817</v>
       </c>
       <c r="G8">
-        <v>4.196158676738227</v>
+        <v>5.430533424785357</v>
       </c>
       <c r="H8">
-        <v>28.79281887351128</v>
+        <v>3.683962949309413</v>
+      </c>
+      <c r="I8">
+        <v>28.4280548726156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>Hispanic</t>
         </is>
       </c>
-      <c r="C9">
-        <v>4.703387344963951</v>
-      </c>
       <c r="D9">
-        <v>13.3255840515091</v>
+        <v>5.174839600101257</v>
       </c>
       <c r="E9">
-        <v>1.987108590042685</v>
+        <v>12.36302340144172</v>
       </c>
       <c r="F9">
-        <v>6.903454256657646</v>
+        <v>1.428578518223841</v>
       </c>
       <c r="G9">
-        <v>5.25270401146703</v>
+        <v>6.998925201952798</v>
       </c>
       <c r="H9">
-        <v>32.17223825464041</v>
+        <v>4.632731230855415</v>
+      </c>
+      <c r="I9">
+        <v>30.59809795257503</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>Hispanic</t>
         </is>
       </c>
-      <c r="C10">
+      <c r="D10">
+        <v>7.32261053673684</v>
+      </c>
+      <c r="E10">
+        <v>11.78680117593682</v>
+      </c>
+      <c r="F10">
+        <v>1.297200430941462</v>
+      </c>
+      <c r="G10">
+        <v>10.11497000523823</v>
+      </c>
+      <c r="H10">
+        <v>3.849342993720903</v>
+      </c>
+      <c r="I10">
+        <v>34.37092514257426</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>3.366303623731205</v>
+      </c>
+      <c r="E11">
+        <v>12.15714401385543</v>
+      </c>
+      <c r="F11">
+        <v>1.737188663037162</v>
+      </c>
+      <c r="G11">
+        <v>4.004564280816123</v>
+      </c>
+      <c r="H11">
+        <v>3.652049221412493</v>
+      </c>
+      <c r="I11">
+        <v>24.91724980285242</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>4.686592407434943</v>
+      </c>
+      <c r="E12">
+        <v>12.74007630712849</v>
+      </c>
+      <c r="F12">
+        <v>1.067978942660879</v>
+      </c>
+      <c r="G12">
+        <v>5.785149508426985</v>
+      </c>
+      <c r="H12">
+        <v>4.629681100983577</v>
+      </c>
+      <c r="I12">
+        <v>28.90947826663487</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>7.655722422417413</v>
+      </c>
+      <c r="E13">
+        <v>11.33642055198433</v>
+      </c>
+      <c r="F13">
+        <v>0.8619887241378588</v>
+      </c>
+      <c r="G13">
+        <v>9.6321956492387</v>
+      </c>
+      <c r="H13">
+        <v>4.461747400534877</v>
+      </c>
+      <c r="I13">
+        <v>33.94807474831318</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>3.056804037521745</v>
+      </c>
+      <c r="E14">
+        <v>11.28969770140409</v>
+      </c>
+      <c r="F14">
+        <v>2.634483856901404</v>
+      </c>
+      <c r="G14">
+        <v>3.383079511480429</v>
+      </c>
+      <c r="H14">
+        <v>2.530826876317968</v>
+      </c>
+      <c r="I14">
+        <v>22.89489198362563</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>4.419344227387025</v>
+      </c>
+      <c r="E15">
+        <v>12.08477614690689</v>
+      </c>
+      <c r="F15">
+        <v>1.72254167945185</v>
+      </c>
+      <c r="G15">
+        <v>5.157664722330637</v>
+      </c>
+      <c r="H15">
+        <v>3.462173094514133</v>
+      </c>
+      <c r="I15">
+        <v>26.84649987059054</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>7.446834057065592</v>
+      </c>
+      <c r="E16">
+        <v>10.79877460733823</v>
+      </c>
+      <c r="F16">
+        <v>1.318006191099182</v>
+      </c>
+      <c r="G16">
+        <v>9.236016582842852</v>
+      </c>
+      <c r="H16">
+        <v>3.629350868742752</v>
+      </c>
+      <c r="I16">
+        <v>32.42898230708861</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>3.510322822902935</v>
+      </c>
+      <c r="E17">
+        <v>12.84694702643727</v>
+      </c>
+      <c r="F17">
+        <v>3.168009596498625</v>
+      </c>
+      <c r="G17">
+        <v>5.071380750934225</v>
+      </c>
+      <c r="H17">
+        <v>4.196158676738227</v>
+      </c>
+      <c r="I17">
+        <v>28.79281887351128</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>4.703387344963951</v>
+      </c>
+      <c r="E18">
+        <v>13.3255840515091</v>
+      </c>
+      <c r="F18">
+        <v>1.987108590042685</v>
+      </c>
+      <c r="G18">
+        <v>6.903454256657646</v>
+      </c>
+      <c r="H18">
+        <v>5.25270401146703</v>
+      </c>
+      <c r="I18">
+        <v>32.17223825464041</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D19">
         <v>7.33472612500473</v>
       </c>
+      <c r="E19">
+        <v>11.70590648267642</v>
+      </c>
+      <c r="F19">
+        <v>1.709671881039287</v>
+      </c>
+      <c r="G19">
+        <v>10.67236643672631</v>
+      </c>
+      <c r="H19">
+        <v>5.045643801293241</v>
+      </c>
+      <c r="I19">
+        <v>36.46831472673999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>retired.healthy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>retired.unhealthy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>not.working</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>working.healthy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>working.unhealthy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>3.621673486831623</v>
+      </c>
+      <c r="E2">
+        <v>11.64050281392282</v>
+      </c>
+      <c r="F2">
+        <v>1.632878664830797</v>
+      </c>
+      <c r="G2">
+        <v>3.810981403678492</v>
+      </c>
+      <c r="H2">
+        <v>3.804620107230797</v>
+      </c>
+      <c r="I2">
+        <v>25.53497920560531</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>5.00653264017557</v>
+      </c>
+      <c r="E3">
+        <v>11.58126334800173</v>
+      </c>
+      <c r="F3">
+        <v>0.8817963560780722</v>
+      </c>
+      <c r="G3">
+        <v>5.130544224359983</v>
+      </c>
+      <c r="H3">
+        <v>4.709607467822759</v>
+      </c>
+      <c r="I3">
+        <v>28.10876169895863</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>7.196382434677743</v>
+      </c>
+      <c r="E4">
+        <v>10.99679775105737</v>
+      </c>
+      <c r="F4">
+        <v>0.633933354425258</v>
+      </c>
+      <c r="G4">
+        <v>7.789017455776307</v>
+      </c>
+      <c r="H4">
+        <v>3.908105438831302</v>
+      </c>
+      <c r="I4">
+        <v>31.90313591500101</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>3.460682449941584</v>
+      </c>
+      <c r="E5">
+        <v>9.652367803148984</v>
+      </c>
+      <c r="F5">
+        <v>2.534624532327719</v>
+      </c>
+      <c r="G5">
+        <v>4.039980515967365</v>
+      </c>
+      <c r="H5">
+        <v>2.165215724535584</v>
+      </c>
+      <c r="I5">
+        <v>23.29930231834405</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>4.77324754640979</v>
+      </c>
+      <c r="E6">
+        <v>9.780881883946035</v>
+      </c>
+      <c r="F6">
+        <v>1.52458162969484</v>
+      </c>
+      <c r="G6">
+        <v>4.967354785117887</v>
+      </c>
+      <c r="H6">
+        <v>2.716588164086312</v>
+      </c>
+      <c r="I6">
+        <v>25.34116157926703</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>7.006537133758249</v>
+      </c>
+      <c r="E7">
+        <v>9.20036377089377</v>
+      </c>
+      <c r="F7">
+        <v>0.8774214895780472</v>
+      </c>
+      <c r="G7">
+        <v>8.118961655433155</v>
+      </c>
+      <c r="H7">
+        <v>2.397619312677774</v>
+      </c>
+      <c r="I7">
+        <v>29.81483726925545</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>3.33027741208477</v>
+      </c>
+      <c r="E8">
+        <v>11.57781780039643</v>
+      </c>
+      <c r="F8">
+        <v>2.401425839482397</v>
+      </c>
+      <c r="G8">
+        <v>4.779320019218368</v>
+      </c>
+      <c r="H8">
+        <v>3.278885755326778</v>
+      </c>
+      <c r="I8">
+        <v>27.3678834155412</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>4.399430320231747</v>
+      </c>
+      <c r="E9">
+        <v>11.29356262709902</v>
+      </c>
+      <c r="F9">
+        <v>1.188388948154997</v>
+      </c>
+      <c r="G9">
+        <v>6.186413181168683</v>
+      </c>
+      <c r="H9">
+        <v>4.076298356878654</v>
+      </c>
+      <c r="I9">
+        <v>29.34085237684774</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
       <c r="D10">
-        <v>11.70590648267642</v>
+        <v>6.327099244064804</v>
       </c>
       <c r="E10">
-        <v>1.709671881039287</v>
+        <v>10.6506450720942</v>
       </c>
       <c r="F10">
-        <v>10.67236643672631</v>
+        <v>0.9179690152437183</v>
       </c>
       <c r="G10">
-        <v>5.045643801293241</v>
+        <v>8.666585393347273</v>
       </c>
       <c r="H10">
-        <v>36.46831472673999</v>
+        <v>3.171198332565996</v>
+      </c>
+      <c r="I10">
+        <v>33.08204966348067</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>2.982533911853617</v>
+      </c>
+      <c r="E11">
+        <v>11.43060328950386</v>
+      </c>
+      <c r="F11">
+        <v>1.507884307349629</v>
+      </c>
+      <c r="G11">
+        <v>3.523668555434116</v>
+      </c>
+      <c r="H11">
+        <v>3.27552841091159</v>
+      </c>
+      <c r="I11">
+        <v>24.0004377478499</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>4.367020297270978</v>
+      </c>
+      <c r="E12">
+        <v>12.2450123851981</v>
+      </c>
+      <c r="F12">
+        <v>0.9509591341518101</v>
+      </c>
+      <c r="G12">
+        <v>5.459370744458218</v>
+      </c>
+      <c r="H12">
+        <v>4.349540939697084</v>
+      </c>
+      <c r="I12">
+        <v>28.24695231565955</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>7.108934049739867</v>
+      </c>
+      <c r="E13">
+        <v>10.72552888691363</v>
+      </c>
+      <c r="F13">
+        <v>0.7304152538434123</v>
+      </c>
+      <c r="G13">
+        <v>9.153418605152192</v>
+      </c>
+      <c r="H13">
+        <v>4.120153448305939</v>
+      </c>
+      <c r="I13">
+        <v>33.18204624239705</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>2.680676592430095</v>
+      </c>
+      <c r="E14">
+        <v>10.37830074866653</v>
+      </c>
+      <c r="F14">
+        <v>2.264011703689122</v>
+      </c>
+      <c r="G14">
+        <v>2.955904089529759</v>
+      </c>
+      <c r="H14">
+        <v>2.204888370346542</v>
+      </c>
+      <c r="I14">
+        <v>21.72335966966821</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>3.887244701796076</v>
+      </c>
+      <c r="E15">
+        <v>11.1678638603009</v>
+      </c>
+      <c r="F15">
+        <v>1.478864184270605</v>
+      </c>
+      <c r="G15">
+        <v>4.707968706522495</v>
+      </c>
+      <c r="H15">
+        <v>3.082574543565896</v>
+      </c>
+      <c r="I15">
+        <v>25.76903208936444</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>6.590979993295177</v>
+      </c>
+      <c r="E16">
+        <v>9.861411499275597</v>
+      </c>
+      <c r="F16">
+        <v>1.063176725844848</v>
+      </c>
+      <c r="G16">
+        <v>8.533649766620872</v>
+      </c>
+      <c r="H16">
+        <v>3.155652354912724</v>
+      </c>
+      <c r="I16">
+        <v>31.30727254268531</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>3.075985297624905</v>
+      </c>
+      <c r="E17">
+        <v>11.95813148424037</v>
+      </c>
+      <c r="F17">
+        <v>2.739613465971768</v>
+      </c>
+      <c r="G17">
+        <v>4.586509543284576</v>
+      </c>
+      <c r="H17">
+        <v>3.776569254198731</v>
+      </c>
+      <c r="I17">
+        <v>27.83334350895432</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>4.180324670746351</v>
+      </c>
+      <c r="E18">
+        <v>12.31697959871009</v>
+      </c>
+      <c r="F18">
+        <v>1.71231557300916</v>
+      </c>
+      <c r="G18">
+        <v>6.301888517003109</v>
+      </c>
+      <c r="H18">
+        <v>4.708746118569282</v>
+      </c>
+      <c r="I18">
+        <v>31.07287831311399</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>6.560502548223248</v>
+      </c>
+      <c r="E19">
+        <v>10.61028329212179</v>
+      </c>
+      <c r="F19">
+        <v>1.373799615400632</v>
+      </c>
+      <c r="G19">
+        <v>9.724924936146996</v>
+      </c>
+      <c r="H19">
+        <v>4.336448733571595</v>
+      </c>
+      <c r="I19">
+        <v>35.38059301543051</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>race</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>retired.healthy</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>retired.unhealthy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>not.working</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>working.healthy</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>working.unhealthy</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>4.197954619911603</v>
+      </c>
+      <c r="E2">
+        <v>12.91603197839357</v>
+      </c>
+      <c r="F2">
+        <v>2.128118768379951</v>
+      </c>
+      <c r="G2">
+        <v>4.521984333043158</v>
+      </c>
+      <c r="H2">
+        <v>4.483816088999347</v>
+      </c>
+      <c r="I2">
+        <v>27.08176502118015</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>5.552275334235405</v>
+      </c>
+      <c r="E3">
+        <v>12.57182363543101</v>
+      </c>
+      <c r="F3">
+        <v>1.106919183687511</v>
+      </c>
+      <c r="G3">
+        <v>5.659483547756013</v>
+      </c>
+      <c r="H3">
+        <v>5.230836742582949</v>
+      </c>
+      <c r="I3">
+        <v>29.23359183381882</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>8.349802723764062</v>
+      </c>
+      <c r="E4">
+        <v>12.33562133867095</v>
+      </c>
+      <c r="F4">
+        <v>0.8806330063962344</v>
+      </c>
+      <c r="G4">
+        <v>8.672447815337836</v>
+      </c>
+      <c r="H4">
+        <v>4.570724251458331</v>
+      </c>
+      <c r="I4">
+        <v>33.40906661789739</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>4.32010229713605</v>
+      </c>
+      <c r="E5">
+        <v>11.32456883974523</v>
+      </c>
+      <c r="F5">
+        <v>3.328952777096485</v>
+      </c>
+      <c r="G5">
+        <v>5.130291578835445</v>
+      </c>
+      <c r="H5">
+        <v>2.86674256659149</v>
+      </c>
+      <c r="I5">
+        <v>25.36213129214302</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>5.979313855502381</v>
+      </c>
+      <c r="E6">
+        <v>11.38921166429401</v>
+      </c>
+      <c r="F6">
+        <v>2.092377658173603</v>
+      </c>
+      <c r="G6">
+        <v>6.203562841176263</v>
+      </c>
+      <c r="H6">
+        <v>3.508906129455279</v>
+      </c>
+      <c r="I6">
+        <v>27.57881447281109</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>8.798567854414653</v>
+      </c>
+      <c r="E7">
+        <v>11.15706922430158</v>
+      </c>
+      <c r="F7">
+        <v>1.457562906317226</v>
+      </c>
+      <c r="G7">
+        <v>9.995211860632292</v>
+      </c>
+      <c r="H7">
+        <v>3.328293896445257</v>
+      </c>
+      <c r="I7">
+        <v>32.21607712683249</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>4.360368092134082</v>
+      </c>
+      <c r="E8">
+        <v>13.63128669115332</v>
+      </c>
+      <c r="F8">
+        <v>3.29033577264115</v>
+      </c>
+      <c r="G8">
+        <v>6.201195474741009</v>
+      </c>
+      <c r="H8">
+        <v>4.134057950223093</v>
+      </c>
+      <c r="I8">
+        <v>29.73405354460072</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>5.836401746752582</v>
+      </c>
+      <c r="E9">
+        <v>13.66894752868324</v>
+      </c>
+      <c r="F9">
+        <v>1.698710141896055</v>
+      </c>
+      <c r="G9">
+        <v>7.940136604754508</v>
+      </c>
+      <c r="H9">
+        <v>5.272868459086143</v>
+      </c>
+      <c r="I9">
+        <v>31.99367922545131</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>8.36404280729243</v>
+      </c>
+      <c r="E10">
+        <v>12.960108887766</v>
+      </c>
+      <c r="F10">
+        <v>1.752960612986624</v>
+      </c>
+      <c r="G10">
+        <v>11.26606329580022</v>
+      </c>
+      <c r="H10">
+        <v>4.483712164622366</v>
+      </c>
+      <c r="I10">
+        <v>35.77569418918486</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>3.810839514845163</v>
+      </c>
+      <c r="E11">
+        <v>12.93066505043811</v>
+      </c>
+      <c r="F11">
+        <v>1.987801927875739</v>
+      </c>
+      <c r="G11">
+        <v>4.5456954421637</v>
+      </c>
+      <c r="H11">
+        <v>4.199701133310081</v>
+      </c>
+      <c r="I11">
+        <v>25.89239120166533</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>5.025672885858662</v>
+      </c>
+      <c r="E12">
+        <v>13.27944510058067</v>
+      </c>
+      <c r="F12">
+        <v>1.1923271789581</v>
+      </c>
+      <c r="G12">
+        <v>6.104014317189105</v>
+      </c>
+      <c r="H12">
+        <v>4.893386520639977</v>
+      </c>
+      <c r="I12">
+        <v>29.62649132365864</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>8.112867523128156</v>
+      </c>
+      <c r="E13">
+        <v>11.92401261932587</v>
+      </c>
+      <c r="F13">
+        <v>1.003432460004418</v>
+      </c>
+      <c r="G13">
+        <v>10.24061741923984</v>
+      </c>
+      <c r="H13">
+        <v>4.815865292907919</v>
+      </c>
+      <c r="I13">
+        <v>34.59639683951585</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>3.420061708375012</v>
+      </c>
+      <c r="E14">
+        <v>12.22397097927271</v>
+      </c>
+      <c r="F14">
+        <v>2.98342615195095</v>
+      </c>
+      <c r="G14">
+        <v>3.895314888971908</v>
+      </c>
+      <c r="H14">
+        <v>2.991826999407154</v>
+      </c>
+      <c r="I14">
+        <v>23.9426013693996</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>4.880181088524324</v>
+      </c>
+      <c r="E15">
+        <v>12.8875402256834</v>
+      </c>
+      <c r="F15">
+        <v>1.934781754969059</v>
+      </c>
+      <c r="G15">
+        <v>5.593489091656313</v>
+      </c>
+      <c r="H15">
+        <v>3.831374168242989</v>
+      </c>
+      <c r="I15">
+        <v>27.88187127104929</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>8.230821042453787</v>
+      </c>
+      <c r="E16">
+        <v>11.68295064487212</v>
+      </c>
+      <c r="F16">
+        <v>1.544937322154876</v>
+      </c>
+      <c r="G16">
+        <v>10.07262411906979</v>
+      </c>
+      <c r="H16">
+        <v>4.089603389344624</v>
+      </c>
+      <c r="I16">
+        <v>33.43876238423223</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>3.94899258643628</v>
+      </c>
+      <c r="E17">
+        <v>13.96675275415976</v>
+      </c>
+      <c r="F17">
+        <v>3.514742996274003</v>
+      </c>
+      <c r="G17">
+        <v>5.68850229460286</v>
+      </c>
+      <c r="H17">
+        <v>4.622755699157404</v>
+      </c>
+      <c r="I17">
+        <v>30.10158836618591</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>5.32054471044072</v>
+      </c>
+      <c r="E18">
+        <v>14.43919134171797</v>
+      </c>
+      <c r="F18">
+        <v>2.2786570273724</v>
+      </c>
+      <c r="G18">
+        <v>7.55164442706731</v>
+      </c>
+      <c r="H18">
+        <v>5.831839274199254</v>
+      </c>
+      <c r="I18">
+        <v>33.38375767090039</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hispanic</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>8.44631213807056</v>
+      </c>
+      <c r="E19">
+        <v>12.76609936117235</v>
+      </c>
+      <c r="F19">
+        <v>2.054992491356983</v>
+      </c>
+      <c r="G19">
+        <v>11.58183231349909</v>
+      </c>
+      <c r="H19">
+        <v>5.724543234939704</v>
+      </c>
+      <c r="I19">
+        <v>37.66605398560591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>